<commit_message>
Update Product Backlog Testing.xlsx
</commit_message>
<xml_diff>
--- a/Product Backlog Testing.xlsx
+++ b/Product Backlog Testing.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>#</t>
   </si>
@@ -31,16 +31,25 @@
     <t>Inform about unit testing</t>
   </si>
   <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>installing necessary software</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create prototypes for unit testing </t>
+  </si>
+  <si>
+    <t>analize diagrams for each component</t>
+  </si>
+  <si>
+    <t>create unit testing for components</t>
+  </si>
+  <si>
     <t>to do</t>
-  </si>
-  <si>
-    <t>installing necessary software</t>
-  </si>
-  <si>
-    <t>analize diagrams for each component</t>
-  </si>
-  <si>
-    <t>create unit testing for components</t>
   </si>
   <si>
     <t>eventual bug/incompatibility identification</t>
@@ -96,7 +105,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -108,6 +117,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -183,7 +195,7 @@
         <v>1.0</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E3" s="3">
         <v>1.0</v>
@@ -191,16 +203,16 @@
     </row>
     <row r="4">
       <c r="A4" s="3">
-        <v>5.0</v>
-      </c>
-      <c r="B4" s="3" t="s">
+        <v>11.0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="E4" s="3">
         <v>1.0</v>
@@ -208,33 +220,33 @@
     </row>
     <row r="5">
       <c r="A5" s="3">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3">
         <v>2.0</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E5" s="3">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3">
         <v>2.0</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E6" s="3">
         <v>3.0</v>
@@ -242,33 +254,33 @@
     </row>
     <row r="7">
       <c r="A7" s="3">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C7" s="3">
         <v>2.0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E7" s="3">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3">
-        <v>2.0</v>
+        <v>8.0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C8" s="3">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E8" s="3">
         <v>2.0</v>
@@ -276,33 +288,33 @@
     </row>
     <row r="9">
       <c r="A9" s="3">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3">
         <v>3.0</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E9" s="3">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3">
-        <v>9.0</v>
+        <v>3.0</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C10" s="3">
         <v>3.0</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E10" s="3">
         <v>1.0</v>
@@ -310,18 +322,35 @@
     </row>
     <row r="11">
       <c r="A11" s="3">
+        <v>9.0</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3">
         <v>10.0</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="3">
+      <c r="B12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="3">
         <v>4.0</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="3">
+      <c r="D12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="3">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>